<commit_message>
added sample json file
</commit_message>
<xml_diff>
--- a/docs/sample-view.xlsx
+++ b/docs/sample-view.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\g0pinath\k8s-secops-reports\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59687150-B766-4DEB-9E44-8202328CBA8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25E66EE7-BAD6-4364-869A-4BD391947E83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{A6655244-6574-4107-B7BA-2DFCA78273D7}"/>
+    <workbookView minimized="1" xWindow="2232" yWindow="2232" windowWidth="17280" windowHeight="9072" xr2:uid="{A6655244-6574-4107-B7BA-2DFCA78273D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="40">
   <si>
     <t>isFullyCompliant</t>
   </si>
@@ -56,9 +56,6 @@
     <t>createdBy</t>
   </si>
   <si>
-    <t>ClusterLevel</t>
-  </si>
-  <si>
     <t>NameSpaceLevel</t>
   </si>
   <si>
@@ -138,6 +135,24 @@
   </si>
   <si>
     <t>Cluster</t>
+  </si>
+  <si>
+    <t>KubeSecurityEvents</t>
+  </si>
+  <si>
+    <t>EventName</t>
+  </si>
+  <si>
+    <t>LoggedonUser</t>
+  </si>
+  <si>
+    <t>TimeGen</t>
+  </si>
+  <si>
+    <t>ClusterLevel(clusterName)</t>
+  </si>
+  <si>
+    <t>policyLastUpdated</t>
   </si>
 </sst>
 </file>
@@ -507,15 +522,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCDB14BF-9E98-482A-85B5-9BA02DB7CE12}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:J10"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="17" bestFit="1" customWidth="1"/>
@@ -527,7 +542,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -539,7 +554,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -559,19 +574,19 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" s="2">
         <v>44321</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G2" s="2">
         <v>44321</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -585,12 +600,12 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>1</v>
@@ -614,7 +629,7 @@
         <v>6</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -625,22 +640,22 @@
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" s="2">
         <v>44321</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H6" s="2">
         <v>44321</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -651,27 +666,27 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" s="2">
         <v>44321</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H7" s="2">
         <v>44321</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>1</v>
@@ -703,22 +718,22 @@
         <v>1</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" s="2">
         <v>44321</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H9" s="2">
         <v>44321</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -729,135 +744,149 @@
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F10" s="2">
         <v>44321</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H10" s="2">
         <v>44321</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="E15" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>21</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>3</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" t="s">
         <v>27</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>28</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" s="3">
+        <v>44321</v>
+      </c>
+      <c r="G16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="3">
-        <v>44321</v>
-      </c>
-      <c r="G16" t="s">
-        <v>24</v>
-      </c>
-      <c r="H16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>30</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" s="3">
+        <v>44321</v>
+      </c>
+      <c r="G17" t="s">
         <v>31</v>
       </c>
-      <c r="E17" t="s">
+      <c r="H17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="3">
-        <v>44321</v>
-      </c>
-      <c r="G17" t="s">
-        <v>32</v>
-      </c>
-      <c r="H17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>30</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="3">
+        <v>44321</v>
+      </c>
+      <c r="G18" t="s">
         <v>31</v>
       </c>
-      <c r="E18" t="s">
-        <v>29</v>
-      </c>
-      <c r="F18" s="3">
-        <v>44321</v>
-      </c>
-      <c r="G18" t="s">
-        <v>32</v>
-      </c>
       <c r="H18" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>